<commit_message>
comments in JFX_GUI.java are back to english again & changes in the Excel-File example.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/example.xlsx
+++ b/src/main/resources/excel/example.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bzzch-my.sharepoint.com/personal/giuntinil_bzz_ch/Documents/Desktop/IMS BZZ/M411/M411-Gruppenarbeit-Gr.-C/src/main/resources/excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{D916DC27-9555-4471-A09D-6F36DFE2B2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3DA9E291-B873-4F38-BA7A-7D7B308218B9}"/>
+  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{D916DC27-9555-4471-A09D-6F36DFE2B2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{674D1F2B-D388-4D45-A33B-E8D5B1724E9A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="350" windowWidth="22780" windowHeight="14800" xr2:uid="{62904B46-200C-4F97-A54A-93A5BE9BE8C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
   <si>
     <t>InversTeilsortiert1000</t>
   </si>
@@ -103,10 +104,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -277,6 +285,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -293,6 +304,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -614,8 +637,8 @@
   </sheetPr>
   <dimension ref="A1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="Q38" sqref="Q38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -637,10 +660,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="10"/>
+      <c r="B1" s="11"/>
       <c r="C1" s="5"/>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -673,8 +696,8 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="5"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -689,78 +712,150 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+      <c r="E3" s="2">
+        <v>2</v>
+      </c>
+      <c r="F3" s="2">
+        <v>3</v>
+      </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
+      <c r="H3" s="9">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>2</v>
+      </c>
+      <c r="J3" s="9">
+        <v>3</v>
+      </c>
       <c r="K3" s="6"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
+      <c r="L3" s="9">
+        <v>1</v>
+      </c>
+      <c r="M3" s="9">
+        <v>2</v>
+      </c>
+      <c r="N3" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="13"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="D4" s="2">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
+      <c r="F4" s="2">
+        <v>6</v>
+      </c>
       <c r="G4" s="7"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
+      <c r="H4" s="9">
+        <v>4</v>
+      </c>
+      <c r="I4" s="9">
+        <v>5</v>
+      </c>
+      <c r="J4" s="9">
+        <v>6</v>
+      </c>
       <c r="K4" s="7"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
+      <c r="L4" s="9">
+        <v>4</v>
+      </c>
+      <c r="M4" s="9">
+        <v>5</v>
+      </c>
+      <c r="N4" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="13"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="7"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="D5" s="2">
+        <v>7</v>
+      </c>
+      <c r="E5" s="2">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2">
+        <v>9</v>
+      </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
+      <c r="H5" s="9">
+        <v>7</v>
+      </c>
+      <c r="I5" s="9">
+        <v>8</v>
+      </c>
+      <c r="J5" s="9">
+        <v>9</v>
+      </c>
       <c r="K5" s="7"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
+      <c r="L5" s="9">
+        <v>7</v>
+      </c>
+      <c r="M5" s="9">
+        <v>8</v>
+      </c>
+      <c r="N5" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="13"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="8"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>2</v>
+      </c>
+      <c r="F6" s="2">
+        <v>3</v>
+      </c>
       <c r="G6" s="8"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="H6" s="9">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>2</v>
+      </c>
+      <c r="J6" s="9">
+        <v>3</v>
+      </c>
       <c r="K6" s="8"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
+      <c r="L6" s="9">
+        <v>1</v>
+      </c>
+      <c r="M6" s="9">
+        <v>2</v>
+      </c>
+      <c r="N6" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:14" ht="10" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
@@ -776,78 +871,150 @@
       <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>9</v>
       </c>
       <c r="C8" s="6"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2</v>
+      </c>
+      <c r="F8" s="9">
+        <v>3</v>
+      </c>
       <c r="G8" s="6"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
+      <c r="H8" s="9">
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>2</v>
+      </c>
+      <c r="J8" s="9">
+        <v>3</v>
+      </c>
       <c r="K8" s="6"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
+      <c r="L8" s="9">
+        <v>1</v>
+      </c>
+      <c r="M8" s="9">
+        <v>2</v>
+      </c>
+      <c r="N8" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="13"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
+      <c r="D9" s="9">
+        <v>4</v>
+      </c>
+      <c r="E9" s="9">
+        <v>5</v>
+      </c>
+      <c r="F9" s="9">
+        <v>6</v>
+      </c>
       <c r="G9" s="7"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
+      <c r="H9" s="9">
+        <v>4</v>
+      </c>
+      <c r="I9" s="9">
+        <v>5</v>
+      </c>
+      <c r="J9" s="9">
+        <v>6</v>
+      </c>
       <c r="K9" s="7"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
+      <c r="L9" s="9">
+        <v>4</v>
+      </c>
+      <c r="M9" s="9">
+        <v>5</v>
+      </c>
+      <c r="N9" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="13"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="D10" s="9">
+        <v>7</v>
+      </c>
+      <c r="E10" s="9">
+        <v>8</v>
+      </c>
+      <c r="F10" s="9">
+        <v>9</v>
+      </c>
       <c r="G10" s="7"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
+      <c r="H10" s="9">
+        <v>7</v>
+      </c>
+      <c r="I10" s="9">
+        <v>8</v>
+      </c>
+      <c r="J10" s="9">
+        <v>9</v>
+      </c>
       <c r="K10" s="7"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
+      <c r="L10" s="9">
+        <v>7</v>
+      </c>
+      <c r="M10" s="9">
+        <v>8</v>
+      </c>
+      <c r="N10" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="13"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="8"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2</v>
+      </c>
+      <c r="F11" s="9">
+        <v>3</v>
+      </c>
       <c r="G11" s="8"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
+      <c r="H11" s="9">
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
+        <v>2</v>
+      </c>
+      <c r="J11" s="9">
+        <v>3</v>
+      </c>
       <c r="K11" s="8"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
+      <c r="L11" s="9">
+        <v>1</v>
+      </c>
+      <c r="M11" s="9">
+        <v>2</v>
+      </c>
+      <c r="N11" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="1:14" ht="10" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
@@ -863,78 +1030,150 @@
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="14" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C13" s="6"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="D13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>2</v>
+      </c>
+      <c r="F13" s="9">
+        <v>3</v>
+      </c>
       <c r="G13" s="6"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
+      <c r="H13" s="9">
+        <v>1</v>
+      </c>
+      <c r="I13" s="9">
+        <v>2</v>
+      </c>
+      <c r="J13" s="9">
+        <v>3</v>
+      </c>
       <c r="K13" s="6"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
+      <c r="L13" s="9">
+        <v>1</v>
+      </c>
+      <c r="M13" s="9">
+        <v>2</v>
+      </c>
+      <c r="N13" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="7"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="D14" s="9">
+        <v>4</v>
+      </c>
+      <c r="E14" s="9">
+        <v>5</v>
+      </c>
+      <c r="F14" s="9">
+        <v>6</v>
+      </c>
       <c r="G14" s="7"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
+      <c r="H14" s="9">
+        <v>4</v>
+      </c>
+      <c r="I14" s="9">
+        <v>5</v>
+      </c>
+      <c r="J14" s="9">
+        <v>6</v>
+      </c>
       <c r="K14" s="7"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
+      <c r="L14" s="9">
+        <v>4</v>
+      </c>
+      <c r="M14" s="9">
+        <v>5</v>
+      </c>
+      <c r="N14" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="7"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="D15" s="9">
+        <v>7</v>
+      </c>
+      <c r="E15" s="9">
+        <v>8</v>
+      </c>
+      <c r="F15" s="9">
+        <v>9</v>
+      </c>
       <c r="G15" s="7"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
+      <c r="H15" s="9">
+        <v>7</v>
+      </c>
+      <c r="I15" s="9">
+        <v>8</v>
+      </c>
+      <c r="J15" s="9">
+        <v>9</v>
+      </c>
       <c r="K15" s="7"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
+      <c r="L15" s="9">
+        <v>7</v>
+      </c>
+      <c r="M15" s="9">
+        <v>8</v>
+      </c>
+      <c r="N15" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="8"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
+        <v>2</v>
+      </c>
+      <c r="F16" s="9">
+        <v>3</v>
+      </c>
       <c r="G16" s="8"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
+      <c r="H16" s="9">
+        <v>1</v>
+      </c>
+      <c r="I16" s="9">
+        <v>2</v>
+      </c>
+      <c r="J16" s="9">
+        <v>3</v>
+      </c>
       <c r="K16" s="8"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
+      <c r="L16" s="9">
+        <v>1</v>
+      </c>
+      <c r="M16" s="9">
+        <v>2</v>
+      </c>
+      <c r="N16" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="1:14" ht="10" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
@@ -950,78 +1189,150 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="14" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C18" s="6"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="D18" s="9">
+        <v>1</v>
+      </c>
+      <c r="E18" s="9">
+        <v>2</v>
+      </c>
+      <c r="F18" s="9">
+        <v>3</v>
+      </c>
       <c r="G18" s="6"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
+      <c r="H18" s="9">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9">
+        <v>2</v>
+      </c>
+      <c r="J18" s="9">
+        <v>3</v>
+      </c>
       <c r="K18" s="6"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
+      <c r="L18" s="9">
+        <v>1</v>
+      </c>
+      <c r="M18" s="9">
+        <v>2</v>
+      </c>
+      <c r="N18" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C19" s="7"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="D19" s="9">
+        <v>4</v>
+      </c>
+      <c r="E19" s="9">
+        <v>5</v>
+      </c>
+      <c r="F19" s="9">
+        <v>6</v>
+      </c>
       <c r="G19" s="7"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
+      <c r="H19" s="9">
+        <v>4</v>
+      </c>
+      <c r="I19" s="9">
+        <v>5</v>
+      </c>
+      <c r="J19" s="9">
+        <v>6</v>
+      </c>
       <c r="K19" s="7"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
+      <c r="L19" s="9">
+        <v>4</v>
+      </c>
+      <c r="M19" s="9">
+        <v>5</v>
+      </c>
+      <c r="N19" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
+      <c r="A20" s="14"/>
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="D20" s="9">
+        <v>7</v>
+      </c>
+      <c r="E20" s="9">
+        <v>8</v>
+      </c>
+      <c r="F20" s="9">
+        <v>9</v>
+      </c>
       <c r="G20" s="7"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
+      <c r="H20" s="9">
+        <v>7</v>
+      </c>
+      <c r="I20" s="9">
+        <v>8</v>
+      </c>
+      <c r="J20" s="9">
+        <v>9</v>
+      </c>
       <c r="K20" s="7"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
+      <c r="L20" s="9">
+        <v>7</v>
+      </c>
+      <c r="M20" s="9">
+        <v>8</v>
+      </c>
+      <c r="N20" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="13"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="8"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="D21" s="9">
+        <v>1</v>
+      </c>
+      <c r="E21" s="9">
+        <v>2</v>
+      </c>
+      <c r="F21" s="9">
+        <v>3</v>
+      </c>
       <c r="G21" s="8"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
+      <c r="H21" s="9">
+        <v>1</v>
+      </c>
+      <c r="I21" s="9">
+        <v>2</v>
+      </c>
+      <c r="J21" s="9">
+        <v>3</v>
+      </c>
       <c r="K21" s="8"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="2"/>
+      <c r="L21" s="9">
+        <v>1</v>
+      </c>
+      <c r="M21" s="9">
+        <v>2</v>
+      </c>
+      <c r="N21" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="22" spans="1:14" ht="10" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
@@ -1037,78 +1348,150 @@
       <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C23" s="6"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
+      <c r="D23" s="9">
+        <v>1</v>
+      </c>
+      <c r="E23" s="9">
+        <v>2</v>
+      </c>
+      <c r="F23" s="9">
+        <v>3</v>
+      </c>
       <c r="G23" s="6"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
+      <c r="H23" s="9">
+        <v>1</v>
+      </c>
+      <c r="I23" s="9">
+        <v>2</v>
+      </c>
+      <c r="J23" s="9">
+        <v>3</v>
+      </c>
       <c r="K23" s="6"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
+      <c r="L23" s="9">
+        <v>1</v>
+      </c>
+      <c r="M23" s="9">
+        <v>2</v>
+      </c>
+      <c r="N23" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="13"/>
+      <c r="A24" s="14"/>
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="D24" s="9">
+        <v>4</v>
+      </c>
+      <c r="E24" s="9">
+        <v>5</v>
+      </c>
+      <c r="F24" s="9">
+        <v>6</v>
+      </c>
       <c r="G24" s="7"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
+      <c r="H24" s="9">
+        <v>4</v>
+      </c>
+      <c r="I24" s="9">
+        <v>5</v>
+      </c>
+      <c r="J24" s="9">
+        <v>6</v>
+      </c>
       <c r="K24" s="7"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
+      <c r="L24" s="9">
+        <v>4</v>
+      </c>
+      <c r="M24" s="9">
+        <v>5</v>
+      </c>
+      <c r="N24" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="13"/>
+      <c r="A25" s="14"/>
       <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="D25" s="9">
+        <v>7</v>
+      </c>
+      <c r="E25" s="9">
+        <v>8</v>
+      </c>
+      <c r="F25" s="9">
+        <v>9</v>
+      </c>
       <c r="G25" s="7"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
-      <c r="J25" s="2"/>
+      <c r="H25" s="9">
+        <v>7</v>
+      </c>
+      <c r="I25" s="9">
+        <v>8</v>
+      </c>
+      <c r="J25" s="9">
+        <v>9</v>
+      </c>
       <c r="K25" s="7"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
-      <c r="N25" s="2"/>
+      <c r="L25" s="9">
+        <v>7</v>
+      </c>
+      <c r="M25" s="9">
+        <v>8</v>
+      </c>
+      <c r="N25" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="13"/>
+      <c r="A26" s="14"/>
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="8"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="D26" s="9">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>2</v>
+      </c>
+      <c r="F26" s="9">
+        <v>3</v>
+      </c>
       <c r="G26" s="8"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
+      <c r="H26" s="9">
+        <v>1</v>
+      </c>
+      <c r="I26" s="9">
+        <v>2</v>
+      </c>
+      <c r="J26" s="9">
+        <v>3</v>
+      </c>
       <c r="K26" s="8"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="L26" s="9">
+        <v>1</v>
+      </c>
+      <c r="M26" s="9">
+        <v>2</v>
+      </c>
+      <c r="N26" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="27" spans="1:14" ht="10" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
@@ -1124,78 +1507,150 @@
       <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C28" s="6"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
+      <c r="D28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>2</v>
+      </c>
+      <c r="F28" s="9">
+        <v>3</v>
+      </c>
       <c r="G28" s="6"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
-      <c r="J28" s="2"/>
+      <c r="H28" s="9">
+        <v>1</v>
+      </c>
+      <c r="I28" s="9">
+        <v>2</v>
+      </c>
+      <c r="J28" s="9">
+        <v>3</v>
+      </c>
       <c r="K28" s="6"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
-      <c r="N28" s="2"/>
+      <c r="L28" s="9">
+        <v>1</v>
+      </c>
+      <c r="M28" s="9">
+        <v>2</v>
+      </c>
+      <c r="N28" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="13"/>
+      <c r="A29" s="14"/>
       <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C29" s="7"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="D29" s="9">
+        <v>4</v>
+      </c>
+      <c r="E29" s="9">
+        <v>5</v>
+      </c>
+      <c r="F29" s="9">
+        <v>6</v>
+      </c>
       <c r="G29" s="7"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
+      <c r="H29" s="9">
+        <v>4</v>
+      </c>
+      <c r="I29" s="9">
+        <v>5</v>
+      </c>
+      <c r="J29" s="9">
+        <v>6</v>
+      </c>
       <c r="K29" s="7"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
+      <c r="L29" s="9">
+        <v>4</v>
+      </c>
+      <c r="M29" s="9">
+        <v>5</v>
+      </c>
+      <c r="N29" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="13"/>
+      <c r="A30" s="14"/>
       <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C30" s="7"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="D30" s="9">
+        <v>7</v>
+      </c>
+      <c r="E30" s="9">
+        <v>8</v>
+      </c>
+      <c r="F30" s="9">
+        <v>9</v>
+      </c>
       <c r="G30" s="7"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
+      <c r="H30" s="9">
+        <v>7</v>
+      </c>
+      <c r="I30" s="9">
+        <v>8</v>
+      </c>
+      <c r="J30" s="9">
+        <v>9</v>
+      </c>
       <c r="K30" s="7"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
+      <c r="L30" s="9">
+        <v>7</v>
+      </c>
+      <c r="M30" s="9">
+        <v>8</v>
+      </c>
+      <c r="N30" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="13"/>
+      <c r="A31" s="14"/>
       <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C31" s="8"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="D31" s="9">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9">
+        <v>2</v>
+      </c>
+      <c r="F31" s="9">
+        <v>3</v>
+      </c>
       <c r="G31" s="8"/>
-      <c r="H31" s="2"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="2"/>
+      <c r="H31" s="9">
+        <v>1</v>
+      </c>
+      <c r="I31" s="9">
+        <v>2</v>
+      </c>
+      <c r="J31" s="9">
+        <v>3</v>
+      </c>
       <c r="K31" s="8"/>
-      <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
-      <c r="N31" s="2"/>
+      <c r="L31" s="9">
+        <v>1</v>
+      </c>
+      <c r="M31" s="9">
+        <v>2</v>
+      </c>
+      <c r="N31" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:14" ht="10" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
@@ -1211,78 +1666,150 @@
       <c r="N32" s="5"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C33" s="6"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
+      <c r="D33" s="9">
+        <v>1</v>
+      </c>
+      <c r="E33" s="9">
+        <v>2</v>
+      </c>
+      <c r="F33" s="9">
+        <v>3</v>
+      </c>
       <c r="G33" s="6"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
+      <c r="H33" s="9">
+        <v>1</v>
+      </c>
+      <c r="I33" s="9">
+        <v>2</v>
+      </c>
+      <c r="J33" s="9">
+        <v>3</v>
+      </c>
       <c r="K33" s="6"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
+      <c r="L33" s="9">
+        <v>1</v>
+      </c>
+      <c r="M33" s="9">
+        <v>2</v>
+      </c>
+      <c r="N33" s="9">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C34" s="7"/>
-      <c r="D34" s="2"/>
-      <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
+      <c r="D34" s="9">
+        <v>4</v>
+      </c>
+      <c r="E34" s="9">
+        <v>5</v>
+      </c>
+      <c r="F34" s="9">
+        <v>6</v>
+      </c>
       <c r="G34" s="7"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
+      <c r="H34" s="9">
+        <v>4</v>
+      </c>
+      <c r="I34" s="9">
+        <v>5</v>
+      </c>
+      <c r="J34" s="9">
+        <v>6</v>
+      </c>
       <c r="K34" s="7"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
+      <c r="L34" s="9">
+        <v>4</v>
+      </c>
+      <c r="M34" s="9">
+        <v>5</v>
+      </c>
+      <c r="N34" s="9">
+        <v>6</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C35" s="7"/>
-      <c r="D35" s="2"/>
-      <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
+      <c r="D35" s="9">
+        <v>7</v>
+      </c>
+      <c r="E35" s="9">
+        <v>8</v>
+      </c>
+      <c r="F35" s="9">
+        <v>9</v>
+      </c>
       <c r="G35" s="7"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
+      <c r="H35" s="9">
+        <v>7</v>
+      </c>
+      <c r="I35" s="9">
+        <v>8</v>
+      </c>
+      <c r="J35" s="9">
+        <v>9</v>
+      </c>
       <c r="K35" s="7"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
+      <c r="L35" s="9">
+        <v>7</v>
+      </c>
+      <c r="M35" s="9">
+        <v>8</v>
+      </c>
+      <c r="N35" s="9">
+        <v>9</v>
+      </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="8"/>
-      <c r="D36" s="2"/>
-      <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
+      <c r="D36" s="9">
+        <v>1</v>
+      </c>
+      <c r="E36" s="9">
+        <v>2</v>
+      </c>
+      <c r="F36" s="9">
+        <v>3</v>
+      </c>
       <c r="G36" s="8"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
+      <c r="H36" s="9">
+        <v>1</v>
+      </c>
+      <c r="I36" s="9">
+        <v>2</v>
+      </c>
+      <c r="J36" s="9">
+        <v>3</v>
+      </c>
       <c r="K36" s="8"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
+      <c r="L36" s="9">
+        <v>1</v>
+      </c>
+      <c r="M36" s="9">
+        <v>2</v>
+      </c>
+      <c r="N36" s="9">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1298,4 +1825,1013 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="71" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E7ECE7-34A4-4BA8-8D5E-CB0DE6408435}">
+  <dimension ref="A1:K29"/>
+  <sheetViews>
+    <sheetView zoomScale="98" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.08984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.90625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A1" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="16">
+        <v>1</v>
+      </c>
+      <c r="D2" s="17">
+        <v>2</v>
+      </c>
+      <c r="E2" s="17">
+        <v>3</v>
+      </c>
+      <c r="F2" s="16">
+        <v>1</v>
+      </c>
+      <c r="G2" s="17">
+        <v>2</v>
+      </c>
+      <c r="H2" s="17">
+        <v>3</v>
+      </c>
+      <c r="I2" s="16">
+        <v>1</v>
+      </c>
+      <c r="J2" s="17">
+        <v>2</v>
+      </c>
+      <c r="K2" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="14"/>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="18">
+        <v>4</v>
+      </c>
+      <c r="D3" s="19">
+        <v>5</v>
+      </c>
+      <c r="E3" s="19">
+        <v>6</v>
+      </c>
+      <c r="F3" s="18">
+        <v>4</v>
+      </c>
+      <c r="G3" s="19">
+        <v>5</v>
+      </c>
+      <c r="H3" s="19">
+        <v>6</v>
+      </c>
+      <c r="I3" s="18">
+        <v>4</v>
+      </c>
+      <c r="J3" s="19">
+        <v>5</v>
+      </c>
+      <c r="K3" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="14"/>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="18">
+        <v>7</v>
+      </c>
+      <c r="D4" s="19">
+        <v>8</v>
+      </c>
+      <c r="E4" s="19">
+        <v>9</v>
+      </c>
+      <c r="F4" s="18">
+        <v>7</v>
+      </c>
+      <c r="G4" s="19">
+        <v>8</v>
+      </c>
+      <c r="H4" s="19">
+        <v>9</v>
+      </c>
+      <c r="I4" s="18">
+        <v>7</v>
+      </c>
+      <c r="J4" s="19">
+        <v>8</v>
+      </c>
+      <c r="K4" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="14"/>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19">
+        <v>2</v>
+      </c>
+      <c r="E5" s="19">
+        <v>3</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1</v>
+      </c>
+      <c r="G5" s="19">
+        <v>2</v>
+      </c>
+      <c r="H5" s="19">
+        <v>3</v>
+      </c>
+      <c r="I5" s="18">
+        <v>1</v>
+      </c>
+      <c r="J5" s="19">
+        <v>2</v>
+      </c>
+      <c r="K5" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="17">
+        <v>2</v>
+      </c>
+      <c r="E6" s="17">
+        <v>3</v>
+      </c>
+      <c r="F6" s="16">
+        <v>1</v>
+      </c>
+      <c r="G6" s="17">
+        <v>2</v>
+      </c>
+      <c r="H6" s="17">
+        <v>3</v>
+      </c>
+      <c r="I6" s="16">
+        <v>1</v>
+      </c>
+      <c r="J6" s="17">
+        <v>2</v>
+      </c>
+      <c r="K6" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="14"/>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="18">
+        <v>4</v>
+      </c>
+      <c r="D7" s="19">
+        <v>5</v>
+      </c>
+      <c r="E7" s="19">
+        <v>6</v>
+      </c>
+      <c r="F7" s="18">
+        <v>4</v>
+      </c>
+      <c r="G7" s="19">
+        <v>5</v>
+      </c>
+      <c r="H7" s="19">
+        <v>6</v>
+      </c>
+      <c r="I7" s="18">
+        <v>4</v>
+      </c>
+      <c r="J7" s="19">
+        <v>5</v>
+      </c>
+      <c r="K7" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
+      <c r="B8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="18">
+        <v>7</v>
+      </c>
+      <c r="D8" s="19">
+        <v>8</v>
+      </c>
+      <c r="E8" s="19">
+        <v>9</v>
+      </c>
+      <c r="F8" s="18">
+        <v>7</v>
+      </c>
+      <c r="G8" s="19">
+        <v>8</v>
+      </c>
+      <c r="H8" s="19">
+        <v>9</v>
+      </c>
+      <c r="I8" s="18">
+        <v>7</v>
+      </c>
+      <c r="J8" s="19">
+        <v>8</v>
+      </c>
+      <c r="K8" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="14"/>
+      <c r="B9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="18">
+        <v>1</v>
+      </c>
+      <c r="D9" s="19">
+        <v>2</v>
+      </c>
+      <c r="E9" s="19">
+        <v>3</v>
+      </c>
+      <c r="F9" s="18">
+        <v>1</v>
+      </c>
+      <c r="G9" s="19">
+        <v>2</v>
+      </c>
+      <c r="H9" s="19">
+        <v>3</v>
+      </c>
+      <c r="I9" s="18">
+        <v>1</v>
+      </c>
+      <c r="J9" s="19">
+        <v>2</v>
+      </c>
+      <c r="K9" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="17">
+        <v>2</v>
+      </c>
+      <c r="E10" s="17">
+        <v>3</v>
+      </c>
+      <c r="F10" s="16">
+        <v>1</v>
+      </c>
+      <c r="G10" s="17">
+        <v>2</v>
+      </c>
+      <c r="H10" s="17">
+        <v>3</v>
+      </c>
+      <c r="I10" s="16">
+        <v>1</v>
+      </c>
+      <c r="J10" s="17">
+        <v>2</v>
+      </c>
+      <c r="K10" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="14"/>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="18">
+        <v>4</v>
+      </c>
+      <c r="D11" s="19">
+        <v>5</v>
+      </c>
+      <c r="E11" s="19">
+        <v>6</v>
+      </c>
+      <c r="F11" s="18">
+        <v>4</v>
+      </c>
+      <c r="G11" s="19">
+        <v>5</v>
+      </c>
+      <c r="H11" s="19">
+        <v>6</v>
+      </c>
+      <c r="I11" s="18">
+        <v>4</v>
+      </c>
+      <c r="J11" s="19">
+        <v>5</v>
+      </c>
+      <c r="K11" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12" s="14"/>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="18">
+        <v>7</v>
+      </c>
+      <c r="D12" s="19">
+        <v>8</v>
+      </c>
+      <c r="E12" s="19">
+        <v>9</v>
+      </c>
+      <c r="F12" s="18">
+        <v>7</v>
+      </c>
+      <c r="G12" s="19">
+        <v>8</v>
+      </c>
+      <c r="H12" s="19">
+        <v>9</v>
+      </c>
+      <c r="I12" s="18">
+        <v>7</v>
+      </c>
+      <c r="J12" s="19">
+        <v>8</v>
+      </c>
+      <c r="K12" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="14"/>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="18">
+        <v>1</v>
+      </c>
+      <c r="D13" s="19">
+        <v>2</v>
+      </c>
+      <c r="E13" s="19">
+        <v>3</v>
+      </c>
+      <c r="F13" s="18">
+        <v>1</v>
+      </c>
+      <c r="G13" s="19">
+        <v>2</v>
+      </c>
+      <c r="H13" s="19">
+        <v>3</v>
+      </c>
+      <c r="I13" s="18">
+        <v>1</v>
+      </c>
+      <c r="J13" s="19">
+        <v>2</v>
+      </c>
+      <c r="K13" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="17">
+        <v>2</v>
+      </c>
+      <c r="E14" s="17">
+        <v>3</v>
+      </c>
+      <c r="F14" s="16">
+        <v>1</v>
+      </c>
+      <c r="G14" s="17">
+        <v>2</v>
+      </c>
+      <c r="H14" s="17">
+        <v>3</v>
+      </c>
+      <c r="I14" s="16">
+        <v>1</v>
+      </c>
+      <c r="J14" s="17">
+        <v>2</v>
+      </c>
+      <c r="K14" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="14"/>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="18">
+        <v>4</v>
+      </c>
+      <c r="D15" s="19">
+        <v>5</v>
+      </c>
+      <c r="E15" s="19">
+        <v>6</v>
+      </c>
+      <c r="F15" s="18">
+        <v>4</v>
+      </c>
+      <c r="G15" s="19">
+        <v>5</v>
+      </c>
+      <c r="H15" s="19">
+        <v>6</v>
+      </c>
+      <c r="I15" s="18">
+        <v>4</v>
+      </c>
+      <c r="J15" s="19">
+        <v>5</v>
+      </c>
+      <c r="K15" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="14"/>
+      <c r="B16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="18">
+        <v>7</v>
+      </c>
+      <c r="D16" s="19">
+        <v>8</v>
+      </c>
+      <c r="E16" s="19">
+        <v>9</v>
+      </c>
+      <c r="F16" s="18">
+        <v>7</v>
+      </c>
+      <c r="G16" s="19">
+        <v>8</v>
+      </c>
+      <c r="H16" s="19">
+        <v>9</v>
+      </c>
+      <c r="I16" s="18">
+        <v>7</v>
+      </c>
+      <c r="J16" s="19">
+        <v>8</v>
+      </c>
+      <c r="K16" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A17" s="14"/>
+      <c r="B17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="18">
+        <v>1</v>
+      </c>
+      <c r="D17" s="19">
+        <v>2</v>
+      </c>
+      <c r="E17" s="19">
+        <v>3</v>
+      </c>
+      <c r="F17" s="18">
+        <v>1</v>
+      </c>
+      <c r="G17" s="19">
+        <v>2</v>
+      </c>
+      <c r="H17" s="19">
+        <v>3</v>
+      </c>
+      <c r="I17" s="18">
+        <v>1</v>
+      </c>
+      <c r="J17" s="19">
+        <v>2</v>
+      </c>
+      <c r="K17" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="16">
+        <v>1</v>
+      </c>
+      <c r="D18" s="17">
+        <v>2</v>
+      </c>
+      <c r="E18" s="17">
+        <v>3</v>
+      </c>
+      <c r="F18" s="16">
+        <v>1</v>
+      </c>
+      <c r="G18" s="17">
+        <v>2</v>
+      </c>
+      <c r="H18" s="17">
+        <v>3</v>
+      </c>
+      <c r="I18" s="16">
+        <v>1</v>
+      </c>
+      <c r="J18" s="17">
+        <v>2</v>
+      </c>
+      <c r="K18" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19" s="14"/>
+      <c r="B19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19" s="18">
+        <v>4</v>
+      </c>
+      <c r="D19" s="19">
+        <v>5</v>
+      </c>
+      <c r="E19" s="19">
+        <v>6</v>
+      </c>
+      <c r="F19" s="18">
+        <v>4</v>
+      </c>
+      <c r="G19" s="19">
+        <v>5</v>
+      </c>
+      <c r="H19" s="19">
+        <v>6</v>
+      </c>
+      <c r="I19" s="18">
+        <v>4</v>
+      </c>
+      <c r="J19" s="19">
+        <v>5</v>
+      </c>
+      <c r="K19" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20" s="14"/>
+      <c r="B20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" s="18">
+        <v>7</v>
+      </c>
+      <c r="D20" s="19">
+        <v>8</v>
+      </c>
+      <c r="E20" s="19">
+        <v>9</v>
+      </c>
+      <c r="F20" s="18">
+        <v>7</v>
+      </c>
+      <c r="G20" s="19">
+        <v>8</v>
+      </c>
+      <c r="H20" s="19">
+        <v>9</v>
+      </c>
+      <c r="I20" s="18">
+        <v>7</v>
+      </c>
+      <c r="J20" s="19">
+        <v>8</v>
+      </c>
+      <c r="K20" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21" s="14"/>
+      <c r="B21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="18">
+        <v>1</v>
+      </c>
+      <c r="D21" s="19">
+        <v>2</v>
+      </c>
+      <c r="E21" s="19">
+        <v>3</v>
+      </c>
+      <c r="F21" s="18">
+        <v>1</v>
+      </c>
+      <c r="G21" s="19">
+        <v>2</v>
+      </c>
+      <c r="H21" s="19">
+        <v>3</v>
+      </c>
+      <c r="I21" s="18">
+        <v>1</v>
+      </c>
+      <c r="J21" s="19">
+        <v>2</v>
+      </c>
+      <c r="K21" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="16">
+        <v>1</v>
+      </c>
+      <c r="D22" s="17">
+        <v>2</v>
+      </c>
+      <c r="E22" s="17">
+        <v>3</v>
+      </c>
+      <c r="F22" s="16">
+        <v>1</v>
+      </c>
+      <c r="G22" s="17">
+        <v>2</v>
+      </c>
+      <c r="H22" s="17">
+        <v>3</v>
+      </c>
+      <c r="I22" s="16">
+        <v>1</v>
+      </c>
+      <c r="J22" s="17">
+        <v>2</v>
+      </c>
+      <c r="K22" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23" s="14"/>
+      <c r="B23" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C23" s="18">
+        <v>4</v>
+      </c>
+      <c r="D23" s="19">
+        <v>5</v>
+      </c>
+      <c r="E23" s="19">
+        <v>6</v>
+      </c>
+      <c r="F23" s="18">
+        <v>4</v>
+      </c>
+      <c r="G23" s="19">
+        <v>5</v>
+      </c>
+      <c r="H23" s="19">
+        <v>6</v>
+      </c>
+      <c r="I23" s="18">
+        <v>4</v>
+      </c>
+      <c r="J23" s="19">
+        <v>5</v>
+      </c>
+      <c r="K23" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24" s="14"/>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="18">
+        <v>7</v>
+      </c>
+      <c r="D24" s="19">
+        <v>8</v>
+      </c>
+      <c r="E24" s="19">
+        <v>9</v>
+      </c>
+      <c r="F24" s="18">
+        <v>7</v>
+      </c>
+      <c r="G24" s="19">
+        <v>8</v>
+      </c>
+      <c r="H24" s="19">
+        <v>9</v>
+      </c>
+      <c r="I24" s="18">
+        <v>7</v>
+      </c>
+      <c r="J24" s="19">
+        <v>8</v>
+      </c>
+      <c r="K24" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25" s="14"/>
+      <c r="B25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="18">
+        <v>1</v>
+      </c>
+      <c r="D25" s="19">
+        <v>2</v>
+      </c>
+      <c r="E25" s="19">
+        <v>3</v>
+      </c>
+      <c r="F25" s="18">
+        <v>1</v>
+      </c>
+      <c r="G25" s="19">
+        <v>2</v>
+      </c>
+      <c r="H25" s="19">
+        <v>3</v>
+      </c>
+      <c r="I25" s="18">
+        <v>1</v>
+      </c>
+      <c r="J25" s="19">
+        <v>2</v>
+      </c>
+      <c r="K25" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="16">
+        <v>1</v>
+      </c>
+      <c r="D26" s="17">
+        <v>2</v>
+      </c>
+      <c r="E26" s="17">
+        <v>3</v>
+      </c>
+      <c r="F26" s="16">
+        <v>1</v>
+      </c>
+      <c r="G26" s="17">
+        <v>2</v>
+      </c>
+      <c r="H26" s="17">
+        <v>3</v>
+      </c>
+      <c r="I26" s="16">
+        <v>1</v>
+      </c>
+      <c r="J26" s="17">
+        <v>2</v>
+      </c>
+      <c r="K26" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27" s="14"/>
+      <c r="B27" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="18">
+        <v>4</v>
+      </c>
+      <c r="D27" s="19">
+        <v>5</v>
+      </c>
+      <c r="E27" s="19">
+        <v>6</v>
+      </c>
+      <c r="F27" s="18">
+        <v>4</v>
+      </c>
+      <c r="G27" s="19">
+        <v>5</v>
+      </c>
+      <c r="H27" s="19">
+        <v>6</v>
+      </c>
+      <c r="I27" s="18">
+        <v>4</v>
+      </c>
+      <c r="J27" s="19">
+        <v>5</v>
+      </c>
+      <c r="K27" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28" s="14"/>
+      <c r="B28" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="18">
+        <v>7</v>
+      </c>
+      <c r="D28" s="19">
+        <v>8</v>
+      </c>
+      <c r="E28" s="19">
+        <v>9</v>
+      </c>
+      <c r="F28" s="18">
+        <v>7</v>
+      </c>
+      <c r="G28" s="19">
+        <v>8</v>
+      </c>
+      <c r="H28" s="19">
+        <v>9</v>
+      </c>
+      <c r="I28" s="18">
+        <v>7</v>
+      </c>
+      <c r="J28" s="19">
+        <v>8</v>
+      </c>
+      <c r="K28" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29" s="14"/>
+      <c r="B29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C29" s="18">
+        <v>1</v>
+      </c>
+      <c r="D29" s="19">
+        <v>2</v>
+      </c>
+      <c r="E29" s="19">
+        <v>3</v>
+      </c>
+      <c r="F29" s="18">
+        <v>1</v>
+      </c>
+      <c r="G29" s="19">
+        <v>2</v>
+      </c>
+      <c r="H29" s="19">
+        <v>3</v>
+      </c>
+      <c r="I29" s="18">
+        <v>1</v>
+      </c>
+      <c r="J29" s="19">
+        <v>2</v>
+      </c>
+      <c r="K29" s="19">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A26:A29"/>
+    <mergeCell ref="A18:A21"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+    <mergeCell ref="A22:A25"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added default constructor to ExcelFile.java & commented in JFX_GUI.java
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/example.xlsx
+++ b/src/main/resources/excel/example.xlsx
@@ -5,16 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bzzch-my.sharepoint.com/personal/giuntinil_bzz_ch/Documents/Desktop/IMS BZZ/M411/M411-Gruppenarbeit-Gr.-C/src/main/resources/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\OneDrive - Bildungszentrum Zürichsee\Desktop\IMS BZZ\M411\M411-Gruppenarbeit-Gr.-C\src\main\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="154" documentId="13_ncr:1_{D916DC27-9555-4471-A09D-6F36DFE2B2E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{674D1F2B-D388-4D45-A33B-E8D5B1724E9A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DC61316-D8DE-40CB-B0C5-7F19DF38350A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="350" windowWidth="22780" windowHeight="14800" xr2:uid="{62904B46-200C-4F97-A54A-93A5BE9BE8C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="24">
   <si>
     <t>InversTeilsortiert1000</t>
   </si>
@@ -99,6 +99,15 @@
   <si>
     <t>Auswertung</t>
   </si>
+  <si>
+    <t>InsertionSort</t>
+  </si>
+  <si>
+    <t>MergeSort</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
@@ -273,7 +282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -288,6 +297,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -304,18 +317,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -660,10 +661,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="11"/>
+      <c r="B1" s="13"/>
       <c r="C1" s="5"/>
       <c r="D1" s="1" t="s">
         <v>0</v>
@@ -696,8 +697,8 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="7.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="5"/>
       <c r="D2" s="3"/>
       <c r="E2" s="4"/>
@@ -712,7 +713,7 @@
       <c r="N2" s="5"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="8" t="s">
@@ -750,7 +751,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
@@ -786,7 +787,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
@@ -822,7 +823,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
@@ -871,7 +872,7 @@
       <c r="N7" s="5"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -909,7 +910,7 @@
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -945,7 +946,7 @@
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A10" s="14"/>
+      <c r="A10" s="16"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -981,7 +982,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1030,7 +1031,7 @@
       <c r="N12" s="5"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="16" t="s">
         <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
@@ -1068,7 +1069,7 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A14" s="14"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -1104,7 +1105,7 @@
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -1140,7 +1141,7 @@
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -1189,7 +1190,7 @@
       <c r="N17" s="5"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
+      <c r="A18" s="16" t="s">
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
@@ -1227,7 +1228,7 @@
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="1" t="s">
         <v>10</v>
       </c>
@@ -1263,7 +1264,7 @@
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
         <v>11</v>
       </c>
@@ -1299,7 +1300,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="1" t="s">
         <v>12</v>
       </c>
@@ -1348,7 +1349,7 @@
       <c r="N22" s="5"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="16" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1386,7 +1387,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1" t="s">
         <v>10</v>
       </c>
@@ -1422,7 +1423,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1" t="s">
         <v>11</v>
       </c>
@@ -1458,7 +1459,7 @@
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1" t="s">
         <v>12</v>
       </c>
@@ -1507,7 +1508,7 @@
       <c r="N27" s="5"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="16" t="s">
         <v>18</v>
       </c>
       <c r="B28" s="1" t="s">
@@ -1545,7 +1546,7 @@
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
+      <c r="A29" s="16"/>
       <c r="B29" s="1" t="s">
         <v>10</v>
       </c>
@@ -1581,7 +1582,7 @@
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A30" s="14"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="1" t="s">
         <v>11</v>
       </c>
@@ -1617,7 +1618,7 @@
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A31" s="14"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
         <v>12</v>
       </c>
@@ -1666,7 +1667,7 @@
       <c r="N32" s="5"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="16" t="s">
         <v>19</v>
       </c>
       <c r="B33" s="1" t="s">
@@ -1704,7 +1705,7 @@
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A34" s="14"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="1" t="s">
         <v>10</v>
       </c>
@@ -1740,7 +1741,7 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A35" s="14"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="1" t="s">
         <v>11</v>
       </c>
@@ -1776,7 +1777,7 @@
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A36" s="14"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
         <v>12</v>
       </c>
@@ -1828,17 +1829,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E7ECE7-34A4-4BA8-8D5E-CB0DE6408435}">
-  <dimension ref="A1:K29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F58C95-7164-4110-927B-B6CE8D7B5B70}">
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L33" sqref="L33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.36328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="1.81640625" customWidth="1"/>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.08984375" bestFit="1" customWidth="1"/>
@@ -1851,9 +1852,9 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="11"/>
+        <v>9</v>
+      </c>
+      <c r="B1" s="10"/>
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1882,956 +1883,583 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="15" t="s">
+    <row r="2" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="16">
-        <v>1</v>
-      </c>
-      <c r="D2" s="17">
-        <v>2</v>
-      </c>
-      <c r="E2" s="17">
-        <v>3</v>
-      </c>
-      <c r="F2" s="16">
-        <v>1</v>
-      </c>
-      <c r="G2" s="17">
-        <v>2</v>
-      </c>
-      <c r="H2" s="17">
-        <v>3</v>
-      </c>
-      <c r="I2" s="16">
-        <v>1</v>
-      </c>
-      <c r="J2" s="17">
-        <v>2</v>
-      </c>
-      <c r="K2" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="14"/>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="18">
-        <v>4</v>
-      </c>
-      <c r="D3" s="19">
-        <v>5</v>
-      </c>
-      <c r="E3" s="19">
-        <v>6</v>
-      </c>
-      <c r="F3" s="18">
-        <v>4</v>
-      </c>
-      <c r="G3" s="19">
-        <v>5</v>
-      </c>
-      <c r="H3" s="19">
-        <v>6</v>
-      </c>
-      <c r="I3" s="18">
-        <v>4</v>
-      </c>
-      <c r="J3" s="19">
-        <v>5</v>
-      </c>
-      <c r="K3" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="14"/>
-      <c r="B4" s="1" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="18">
-        <v>7</v>
-      </c>
-      <c r="D4" s="19">
-        <v>8</v>
-      </c>
-      <c r="E4" s="19">
-        <v>9</v>
-      </c>
-      <c r="F4" s="18">
-        <v>7</v>
-      </c>
-      <c r="G4" s="19">
-        <v>8</v>
-      </c>
-      <c r="H4" s="19">
-        <v>9</v>
-      </c>
-      <c r="I4" s="18">
-        <v>7</v>
-      </c>
-      <c r="J4" s="19">
-        <v>8</v>
-      </c>
-      <c r="K4" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="14"/>
-      <c r="B5" s="1" t="s">
+      <c r="B21" s="11"/>
+      <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="10"/>
+      <c r="B22" s="10"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="18">
-        <v>1</v>
-      </c>
-      <c r="D5" s="19">
-        <v>2</v>
-      </c>
-      <c r="E5" s="19">
-        <v>3</v>
-      </c>
-      <c r="F5" s="18">
-        <v>1</v>
-      </c>
-      <c r="G5" s="19">
-        <v>2</v>
-      </c>
-      <c r="H5" s="19">
-        <v>3</v>
-      </c>
-      <c r="I5" s="18">
-        <v>1</v>
-      </c>
-      <c r="J5" s="19">
-        <v>2</v>
-      </c>
-      <c r="K5" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="15" t="s">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="10" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="10"/>
+      <c r="B32" s="10"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="16">
-        <v>1</v>
-      </c>
-      <c r="D6" s="17">
-        <v>2</v>
-      </c>
-      <c r="E6" s="17">
-        <v>3</v>
-      </c>
-      <c r="F6" s="16">
-        <v>1</v>
-      </c>
-      <c r="G6" s="17">
-        <v>2</v>
-      </c>
-      <c r="H6" s="17">
-        <v>3</v>
-      </c>
-      <c r="I6" s="16">
-        <v>1</v>
-      </c>
-      <c r="J6" s="17">
-        <v>2</v>
-      </c>
-      <c r="K6" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="14"/>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="18">
-        <v>4</v>
-      </c>
-      <c r="D7" s="19">
-        <v>5</v>
-      </c>
-      <c r="E7" s="19">
-        <v>6</v>
-      </c>
-      <c r="F7" s="18">
-        <v>4</v>
-      </c>
-      <c r="G7" s="19">
-        <v>5</v>
-      </c>
-      <c r="H7" s="19">
-        <v>6</v>
-      </c>
-      <c r="I7" s="18">
-        <v>4</v>
-      </c>
-      <c r="J7" s="19">
-        <v>5</v>
-      </c>
-      <c r="K7" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="14"/>
-      <c r="B8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="18">
-        <v>7</v>
-      </c>
-      <c r="D8" s="19">
-        <v>8</v>
-      </c>
-      <c r="E8" s="19">
-        <v>9</v>
-      </c>
-      <c r="F8" s="18">
-        <v>7</v>
-      </c>
-      <c r="G8" s="19">
-        <v>8</v>
-      </c>
-      <c r="H8" s="19">
-        <v>9</v>
-      </c>
-      <c r="I8" s="18">
-        <v>7</v>
-      </c>
-      <c r="J8" s="19">
-        <v>8</v>
-      </c>
-      <c r="K8" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="14"/>
-      <c r="B9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="18">
-        <v>1</v>
-      </c>
-      <c r="D9" s="19">
-        <v>2</v>
-      </c>
-      <c r="E9" s="19">
-        <v>3</v>
-      </c>
-      <c r="F9" s="18">
-        <v>1</v>
-      </c>
-      <c r="G9" s="19">
-        <v>2</v>
-      </c>
-      <c r="H9" s="19">
-        <v>3</v>
-      </c>
-      <c r="I9" s="18">
-        <v>1</v>
-      </c>
-      <c r="J9" s="19">
-        <v>2</v>
-      </c>
-      <c r="K9" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="14" t="s">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="16">
-        <v>1</v>
-      </c>
-      <c r="D10" s="17">
-        <v>2</v>
-      </c>
-      <c r="E10" s="17">
-        <v>3</v>
-      </c>
-      <c r="F10" s="16">
-        <v>1</v>
-      </c>
-      <c r="G10" s="17">
-        <v>2</v>
-      </c>
-      <c r="H10" s="17">
-        <v>3</v>
-      </c>
-      <c r="I10" s="16">
-        <v>1</v>
-      </c>
-      <c r="J10" s="17">
-        <v>2</v>
-      </c>
-      <c r="K10" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="14"/>
-      <c r="B11" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="18">
-        <v>4</v>
-      </c>
-      <c r="D11" s="19">
-        <v>5</v>
-      </c>
-      <c r="E11" s="19">
-        <v>6</v>
-      </c>
-      <c r="F11" s="18">
-        <v>4</v>
-      </c>
-      <c r="G11" s="19">
-        <v>5</v>
-      </c>
-      <c r="H11" s="19">
-        <v>6</v>
-      </c>
-      <c r="I11" s="18">
-        <v>4</v>
-      </c>
-      <c r="J11" s="19">
-        <v>5</v>
-      </c>
-      <c r="K11" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="14"/>
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="18">
-        <v>7</v>
-      </c>
-      <c r="D12" s="19">
-        <v>8</v>
-      </c>
-      <c r="E12" s="19">
-        <v>9</v>
-      </c>
-      <c r="F12" s="18">
-        <v>7</v>
-      </c>
-      <c r="G12" s="19">
-        <v>8</v>
-      </c>
-      <c r="H12" s="19">
-        <v>9</v>
-      </c>
-      <c r="I12" s="18">
-        <v>7</v>
-      </c>
-      <c r="J12" s="19">
-        <v>8</v>
-      </c>
-      <c r="K12" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="18">
-        <v>1</v>
-      </c>
-      <c r="D13" s="19">
-        <v>2</v>
-      </c>
-      <c r="E13" s="19">
-        <v>3</v>
-      </c>
-      <c r="F13" s="18">
-        <v>1</v>
-      </c>
-      <c r="G13" s="19">
-        <v>2</v>
-      </c>
-      <c r="H13" s="19">
-        <v>3</v>
-      </c>
-      <c r="I13" s="18">
-        <v>1</v>
-      </c>
-      <c r="J13" s="19">
-        <v>2</v>
-      </c>
-      <c r="K13" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="16">
-        <v>1</v>
-      </c>
-      <c r="D14" s="17">
-        <v>2</v>
-      </c>
-      <c r="E14" s="17">
-        <v>3</v>
-      </c>
-      <c r="F14" s="16">
-        <v>1</v>
-      </c>
-      <c r="G14" s="17">
-        <v>2</v>
-      </c>
-      <c r="H14" s="17">
-        <v>3</v>
-      </c>
-      <c r="I14" s="16">
-        <v>1</v>
-      </c>
-      <c r="J14" s="17">
-        <v>2</v>
-      </c>
-      <c r="K14" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" s="14"/>
-      <c r="B15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="18">
-        <v>4</v>
-      </c>
-      <c r="D15" s="19">
-        <v>5</v>
-      </c>
-      <c r="E15" s="19">
-        <v>6</v>
-      </c>
-      <c r="F15" s="18">
-        <v>4</v>
-      </c>
-      <c r="G15" s="19">
-        <v>5</v>
-      </c>
-      <c r="H15" s="19">
-        <v>6</v>
-      </c>
-      <c r="I15" s="18">
-        <v>4</v>
-      </c>
-      <c r="J15" s="19">
-        <v>5</v>
-      </c>
-      <c r="K15" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" s="14"/>
-      <c r="B16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="18">
-        <v>7</v>
-      </c>
-      <c r="D16" s="19">
-        <v>8</v>
-      </c>
-      <c r="E16" s="19">
-        <v>9</v>
-      </c>
-      <c r="F16" s="18">
-        <v>7</v>
-      </c>
-      <c r="G16" s="19">
-        <v>8</v>
-      </c>
-      <c r="H16" s="19">
-        <v>9</v>
-      </c>
-      <c r="I16" s="18">
-        <v>7</v>
-      </c>
-      <c r="J16" s="19">
-        <v>8</v>
-      </c>
-      <c r="K16" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" s="14"/>
-      <c r="B17" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="18">
-        <v>1</v>
-      </c>
-      <c r="D17" s="19">
-        <v>2</v>
-      </c>
-      <c r="E17" s="19">
-        <v>3</v>
-      </c>
-      <c r="F17" s="18">
-        <v>1</v>
-      </c>
-      <c r="G17" s="19">
-        <v>2</v>
-      </c>
-      <c r="H17" s="19">
-        <v>3</v>
-      </c>
-      <c r="I17" s="18">
-        <v>1</v>
-      </c>
-      <c r="J17" s="19">
-        <v>2</v>
-      </c>
-      <c r="K17" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="16">
-        <v>1</v>
-      </c>
-      <c r="D18" s="17">
-        <v>2</v>
-      </c>
-      <c r="E18" s="17">
-        <v>3</v>
-      </c>
-      <c r="F18" s="16">
-        <v>1</v>
-      </c>
-      <c r="G18" s="17">
-        <v>2</v>
-      </c>
-      <c r="H18" s="17">
-        <v>3</v>
-      </c>
-      <c r="I18" s="16">
-        <v>1</v>
-      </c>
-      <c r="J18" s="17">
-        <v>2</v>
-      </c>
-      <c r="K18" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="14"/>
-      <c r="B19" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="18">
-        <v>4</v>
-      </c>
-      <c r="D19" s="19">
-        <v>5</v>
-      </c>
-      <c r="E19" s="19">
-        <v>6</v>
-      </c>
-      <c r="F19" s="18">
-        <v>4</v>
-      </c>
-      <c r="G19" s="19">
-        <v>5</v>
-      </c>
-      <c r="H19" s="19">
-        <v>6</v>
-      </c>
-      <c r="I19" s="18">
-        <v>4</v>
-      </c>
-      <c r="J19" s="19">
-        <v>5</v>
-      </c>
-      <c r="K19" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
-      <c r="B20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="18">
-        <v>7</v>
-      </c>
-      <c r="D20" s="19">
-        <v>8</v>
-      </c>
-      <c r="E20" s="19">
-        <v>9</v>
-      </c>
-      <c r="F20" s="18">
-        <v>7</v>
-      </c>
-      <c r="G20" s="19">
-        <v>8</v>
-      </c>
-      <c r="H20" s="19">
-        <v>9</v>
-      </c>
-      <c r="I20" s="18">
-        <v>7</v>
-      </c>
-      <c r="J20" s="19">
-        <v>8</v>
-      </c>
-      <c r="K20" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
-      <c r="B21" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" s="18">
-        <v>1</v>
-      </c>
-      <c r="D21" s="19">
-        <v>2</v>
-      </c>
-      <c r="E21" s="19">
-        <v>3</v>
-      </c>
-      <c r="F21" s="18">
-        <v>1</v>
-      </c>
-      <c r="G21" s="19">
-        <v>2</v>
-      </c>
-      <c r="H21" s="19">
-        <v>3</v>
-      </c>
-      <c r="I21" s="18">
-        <v>1</v>
-      </c>
-      <c r="J21" s="19">
-        <v>2</v>
-      </c>
-      <c r="K21" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="14" t="s">
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="16">
-        <v>1</v>
-      </c>
-      <c r="D22" s="17">
-        <v>2</v>
-      </c>
-      <c r="E22" s="17">
-        <v>3</v>
-      </c>
-      <c r="F22" s="16">
-        <v>1</v>
-      </c>
-      <c r="G22" s="17">
-        <v>2</v>
-      </c>
-      <c r="H22" s="17">
-        <v>3</v>
-      </c>
-      <c r="I22" s="16">
-        <v>1</v>
-      </c>
-      <c r="J22" s="17">
-        <v>2</v>
-      </c>
-      <c r="K22" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="14"/>
-      <c r="B23" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="18">
-        <v>4</v>
-      </c>
-      <c r="D23" s="19">
-        <v>5</v>
-      </c>
-      <c r="E23" s="19">
-        <v>6</v>
-      </c>
-      <c r="F23" s="18">
-        <v>4</v>
-      </c>
-      <c r="G23" s="19">
-        <v>5</v>
-      </c>
-      <c r="H23" s="19">
-        <v>6</v>
-      </c>
-      <c r="I23" s="18">
-        <v>4</v>
-      </c>
-      <c r="J23" s="19">
-        <v>5</v>
-      </c>
-      <c r="K23" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="14"/>
-      <c r="B24" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="18">
-        <v>7</v>
-      </c>
-      <c r="D24" s="19">
-        <v>8</v>
-      </c>
-      <c r="E24" s="19">
-        <v>9</v>
-      </c>
-      <c r="F24" s="18">
-        <v>7</v>
-      </c>
-      <c r="G24" s="19">
-        <v>8</v>
-      </c>
-      <c r="H24" s="19">
-        <v>9</v>
-      </c>
-      <c r="I24" s="18">
-        <v>7</v>
-      </c>
-      <c r="J24" s="19">
-        <v>8</v>
-      </c>
-      <c r="K24" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="14"/>
-      <c r="B25" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="18">
-        <v>1</v>
-      </c>
-      <c r="D25" s="19">
-        <v>2</v>
-      </c>
-      <c r="E25" s="19">
-        <v>3</v>
-      </c>
-      <c r="F25" s="18">
-        <v>1</v>
-      </c>
-      <c r="G25" s="19">
-        <v>2</v>
-      </c>
-      <c r="H25" s="19">
-        <v>3</v>
-      </c>
-      <c r="I25" s="18">
-        <v>1</v>
-      </c>
-      <c r="J25" s="19">
-        <v>2</v>
-      </c>
-      <c r="K25" s="19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="14" t="s">
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="16">
-        <v>1</v>
-      </c>
-      <c r="D26" s="17">
-        <v>2</v>
-      </c>
-      <c r="E26" s="17">
-        <v>3</v>
-      </c>
-      <c r="F26" s="16">
-        <v>1</v>
-      </c>
-      <c r="G26" s="17">
-        <v>2</v>
-      </c>
-      <c r="H26" s="17">
-        <v>3</v>
-      </c>
-      <c r="I26" s="16">
-        <v>1</v>
-      </c>
-      <c r="J26" s="17">
-        <v>2</v>
-      </c>
-      <c r="K26" s="17">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="18">
-        <v>4</v>
-      </c>
-      <c r="D27" s="19">
-        <v>5</v>
-      </c>
-      <c r="E27" s="19">
-        <v>6</v>
-      </c>
-      <c r="F27" s="18">
-        <v>4</v>
-      </c>
-      <c r="G27" s="19">
-        <v>5</v>
-      </c>
-      <c r="H27" s="19">
-        <v>6</v>
-      </c>
-      <c r="I27" s="18">
-        <v>4</v>
-      </c>
-      <c r="J27" s="19">
-        <v>5</v>
-      </c>
-      <c r="K27" s="19">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="14"/>
-      <c r="B28" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="18">
-        <v>7</v>
-      </c>
-      <c r="D28" s="19">
-        <v>8</v>
-      </c>
-      <c r="E28" s="19">
-        <v>9</v>
-      </c>
-      <c r="F28" s="18">
-        <v>7</v>
-      </c>
-      <c r="G28" s="19">
-        <v>8</v>
-      </c>
-      <c r="H28" s="19">
-        <v>9</v>
-      </c>
-      <c r="I28" s="18">
-        <v>7</v>
-      </c>
-      <c r="J28" s="19">
-        <v>8</v>
-      </c>
-      <c r="K28" s="19">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="14"/>
-      <c r="B29" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="18">
-        <v>1</v>
-      </c>
-      <c r="D29" s="19">
-        <v>2</v>
-      </c>
-      <c r="E29" s="19">
-        <v>3</v>
-      </c>
-      <c r="F29" s="18">
-        <v>1</v>
-      </c>
-      <c r="G29" s="19">
-        <v>2</v>
-      </c>
-      <c r="H29" s="19">
-        <v>3</v>
-      </c>
-      <c r="I29" s="18">
-        <v>1</v>
-      </c>
-      <c r="J29" s="19">
-        <v>2</v>
-      </c>
-      <c r="K29" s="19">
-        <v>3</v>
-      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A26:A29"/>
-    <mergeCell ref="A18:A21"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-    <mergeCell ref="A22:A25"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>